<commit_message>
APRIL 8 DAY FIXED NEGATIVE ISSUE
</commit_message>
<xml_diff>
--- a/files/sheet1.xlsx
+++ b/files/sheet1.xlsx
@@ -403,329 +403,329 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2">
-        <v>44274.38541666666</v>
+        <v>44293.38541666666</v>
       </c>
       <c r="B2">
-        <v>14504</v>
+        <v>14745.17529296875</v>
       </c>
       <c r="C2">
-        <v>4425</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2">
-        <v>44274.38542824074</v>
+        <v>44293.38542824074</v>
       </c>
       <c r="B3">
-        <v>14493.2998046875</v>
+        <v>14755</v>
       </c>
       <c r="C3">
-        <v>10800</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2">
-        <v>44274.38543981482</v>
+        <v>44293.38543981482</v>
       </c>
       <c r="B4">
-        <v>14500.5</v>
+        <v>14751</v>
       </c>
       <c r="C4">
-        <v>10425</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
-        <v>44274.38545138889</v>
+        <v>44293.38545138889</v>
       </c>
       <c r="B5">
-        <v>14490</v>
+        <v>14746.2001953125</v>
       </c>
       <c r="C5">
-        <v>7425</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2">
-        <v>44274.38546296296</v>
+        <v>44293.38546296296</v>
       </c>
       <c r="B6">
-        <v>14492.400390625</v>
+        <v>14743.5</v>
       </c>
       <c r="C6">
-        <v>4800</v>
+        <v>5175</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2">
-        <v>44274.38547453703</v>
+        <v>44293.38547453703</v>
       </c>
       <c r="B7">
-        <v>14486.099609375</v>
+        <v>14733</v>
       </c>
       <c r="C7">
-        <v>5025</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2">
-        <v>44274.38548611111</v>
+        <v>44293.38548611111</v>
       </c>
       <c r="B8">
-        <v>14482.400390625</v>
+        <v>14725.0498046875</v>
       </c>
       <c r="C8">
-        <v>4425</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2">
-        <v>44274.38549768519</v>
+        <v>44293.38549768519</v>
       </c>
       <c r="B9">
-        <v>14481.599609375</v>
+        <v>14730.4501953125</v>
       </c>
       <c r="C9">
-        <v>4425</v>
+        <v>975</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2">
-        <v>44274.38550925926</v>
+        <v>44293.38550925926</v>
       </c>
       <c r="B10">
-        <v>14486</v>
+        <v>14724</v>
       </c>
       <c r="C10">
-        <v>2925</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2">
-        <v>44274.38552083333</v>
+        <v>44293.38552083333</v>
       </c>
       <c r="B11">
-        <v>14485.0498046875</v>
+        <v>14718.25</v>
       </c>
       <c r="C11">
-        <v>3000</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2">
-        <v>44274.38553240741</v>
+        <v>44293.38553240741</v>
       </c>
       <c r="B12">
-        <v>14487.099609375</v>
+        <v>14707</v>
       </c>
       <c r="C12">
-        <v>9900</v>
+        <v>6525</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2">
-        <v>44274.38554398148</v>
+        <v>44293.38554398148</v>
       </c>
       <c r="B13">
-        <v>14485.7998046875</v>
+        <v>14706.7001953125</v>
       </c>
       <c r="C13">
-        <v>4425</v>
+        <v>6750</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2">
-        <v>44274.38555555556</v>
+        <v>44293.38555555556</v>
       </c>
       <c r="B14">
-        <v>14487.900390625</v>
+        <v>14704.2001953125</v>
       </c>
       <c r="C14">
-        <v>3600</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2">
-        <v>44274.38556712963</v>
+        <v>44293.38556712963</v>
       </c>
       <c r="B15">
-        <v>14485.25</v>
+        <v>14701</v>
       </c>
       <c r="C15">
-        <v>4500</v>
+        <v>12300</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2">
-        <v>44274.3855787037</v>
+        <v>44293.3855787037</v>
       </c>
       <c r="B16">
-        <v>14485.349609375</v>
+        <v>14708</v>
       </c>
       <c r="C16">
-        <v>4500</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2">
-        <v>44274.38559027778</v>
+        <v>44293.38559027778</v>
       </c>
       <c r="B17">
-        <v>14483.5498046875</v>
+        <v>14710.599609375</v>
       </c>
       <c r="C17">
-        <v>6600</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2">
-        <v>44274.38560185185</v>
+        <v>44293.38560185185</v>
       </c>
       <c r="B18">
-        <v>14484.849609375</v>
+        <v>14710</v>
       </c>
       <c r="C18">
-        <v>3300</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2">
-        <v>44274.38561342593</v>
+        <v>44293.38561342593</v>
       </c>
       <c r="B19">
-        <v>14484.849609375</v>
+        <v>14716.349609375</v>
       </c>
       <c r="C19">
-        <v>3000</v>
+        <v>5325</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2">
-        <v>44274.385625</v>
+        <v>44293.385625</v>
       </c>
       <c r="B20">
-        <v>14485</v>
+        <v>14715.599609375</v>
       </c>
       <c r="C20">
-        <v>1050</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2">
-        <v>44274.38563657407</v>
+        <v>44293.38563657407</v>
       </c>
       <c r="B21">
-        <v>14484</v>
+        <v>14724.150390625</v>
       </c>
       <c r="C21">
-        <v>1950</v>
+        <v>8850</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2">
-        <v>44274.38564814815</v>
+        <v>44293.38564814815</v>
       </c>
       <c r="B22">
-        <v>14485.5498046875</v>
+        <v>14731.849609375</v>
       </c>
       <c r="C22">
-        <v>975</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2">
-        <v>44274.38565972223</v>
+        <v>44293.38565972223</v>
       </c>
       <c r="B23">
-        <v>14485</v>
+        <v>14732.2998046875</v>
       </c>
       <c r="C23">
-        <v>9600</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2">
-        <v>44274.3856712963</v>
+        <v>44293.3856712963</v>
       </c>
       <c r="B24">
-        <v>14487</v>
+        <v>14729.75</v>
       </c>
       <c r="C24">
-        <v>4575</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2">
-        <v>44274.38568287037</v>
+        <v>44293.38568287037</v>
       </c>
       <c r="B25">
-        <v>14491</v>
+        <v>14724.4501953125</v>
       </c>
       <c r="C25">
-        <v>10425</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2">
-        <v>44274.38569444444</v>
+        <v>44293.38569444444</v>
       </c>
       <c r="B26">
-        <v>14491.849609375</v>
+        <v>14721.099609375</v>
       </c>
       <c r="C26">
-        <v>5850</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2">
-        <v>44274.38570601852</v>
+        <v>44293.38570601852</v>
       </c>
       <c r="B27">
-        <v>14493.599609375</v>
+        <v>14721.349609375</v>
       </c>
       <c r="C27">
-        <v>2325</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2">
-        <v>44274.3857175926</v>
+        <v>44293.3857175926</v>
       </c>
       <c r="B28">
-        <v>14496.7998046875</v>
+        <v>14719.75</v>
       </c>
       <c r="C28">
-        <v>3375</v>
+        <v>3225</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2">
-        <v>44274.38572916666</v>
+        <v>44293.38572916666</v>
       </c>
       <c r="B29">
-        <v>14498.7998046875</v>
+        <v>14719.25</v>
       </c>
       <c r="C29">
-        <v>2100</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2">
-        <v>44274.38574074074</v>
+        <v>44293.38574074074</v>
       </c>
       <c r="B30">
-        <v>14498</v>
+        <v>14720.9501953125</v>
       </c>
       <c r="C30">
-        <v>2475</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2">
-        <v>44274.38575231482</v>
+        <v>44293.38575231482</v>
       </c>
       <c r="B31">
-        <v>14501.599609375</v>
+        <v>14720</v>
       </c>
       <c r="C31">
         <v>3000</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2">
-        <v>44274.38576388889</v>
+        <v>44293.38576388889</v>
       </c>
       <c r="B32">
-        <v>14501.5</v>
+        <v>14722.099609375</v>
       </c>
       <c r="C32">
         <v>2250</v>
@@ -744,659 +744,659 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2">
-        <v>44274.38577546296</v>
+        <v>44293.38577546296</v>
       </c>
       <c r="B33">
-        <v>14503.849609375</v>
+        <v>14730</v>
       </c>
       <c r="C33">
-        <v>3975</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2">
-        <v>44274.38578703703</v>
+        <v>44293.38578703703</v>
       </c>
       <c r="B34">
-        <v>14507</v>
+        <v>14726.5498046875</v>
       </c>
       <c r="C34">
-        <v>4200</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2">
-        <v>44274.38579861111</v>
+        <v>44293.38579861111</v>
       </c>
       <c r="B35">
-        <v>14506.150390625</v>
+        <v>14722.5498046875</v>
       </c>
       <c r="C35">
-        <v>1950</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2">
-        <v>44274.38581018519</v>
+        <v>44293.38581018519</v>
       </c>
       <c r="B36">
-        <v>14510.5</v>
+        <v>14725.0498046875</v>
       </c>
       <c r="C36">
-        <v>1200</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2">
-        <v>44274.38582175926</v>
+        <v>44293.38582175926</v>
       </c>
       <c r="B37">
-        <v>14510.849609375</v>
+        <v>14727.650390625</v>
       </c>
       <c r="C37">
-        <v>6600</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2">
-        <v>44274.38583333333</v>
+        <v>44293.38583333333</v>
       </c>
       <c r="B38">
-        <v>14510</v>
+        <v>14730.7998046875</v>
       </c>
       <c r="C38">
-        <v>5550</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2">
-        <v>44274.38584490741</v>
+        <v>44293.38584490741</v>
       </c>
       <c r="B39">
-        <v>14510</v>
+        <v>14727.75</v>
       </c>
       <c r="C39">
-        <v>2250</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2">
-        <v>44274.38585648148</v>
+        <v>44293.38585648148</v>
       </c>
       <c r="B40">
-        <v>14510.9501953125</v>
+        <v>14727.5</v>
       </c>
       <c r="C40">
-        <v>6075</v>
+        <v>525</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2">
-        <v>44274.38586805556</v>
+        <v>44293.38586805556</v>
       </c>
       <c r="B41">
-        <v>14509.5</v>
+        <v>14727.650390625</v>
       </c>
       <c r="C41">
-        <v>1800</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2">
-        <v>44274.38587962963</v>
+        <v>44293.38587962963</v>
       </c>
       <c r="B42">
-        <v>14508.5498046875</v>
+        <v>14730.150390625</v>
       </c>
       <c r="C42">
-        <v>1725</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2">
-        <v>44274.3858912037</v>
+        <v>44293.3858912037</v>
       </c>
       <c r="B43">
-        <v>14504.400390625</v>
+        <v>14730.75</v>
       </c>
       <c r="C43">
-        <v>8475</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2">
-        <v>44274.38590277778</v>
+        <v>44293.38590277778</v>
       </c>
       <c r="B44">
-        <v>14502</v>
+        <v>14730.599609375</v>
       </c>
       <c r="C44">
-        <v>2625</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2">
-        <v>44274.38591435185</v>
+        <v>44293.38591435185</v>
       </c>
       <c r="B45">
-        <v>14500</v>
+        <v>14731.7998046875</v>
       </c>
       <c r="C45">
-        <v>4800</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2">
-        <v>44274.38592592593</v>
+        <v>44293.38592592593</v>
       </c>
       <c r="B46">
-        <v>14501.2998046875</v>
+        <v>14733.5</v>
       </c>
       <c r="C46">
-        <v>1125</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2">
-        <v>44274.3859375</v>
+        <v>44293.3859375</v>
       </c>
       <c r="B47">
-        <v>14500</v>
+        <v>14732.7001953125</v>
       </c>
       <c r="C47">
-        <v>2625</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2">
-        <v>44274.38594907407</v>
+        <v>44293.38594907407</v>
       </c>
       <c r="B48">
-        <v>14499</v>
+        <v>14735.25</v>
       </c>
       <c r="C48">
-        <v>6075</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2">
-        <v>44274.38596064815</v>
+        <v>44293.38596064815</v>
       </c>
       <c r="B49">
-        <v>14500.849609375</v>
+        <v>14738.5</v>
       </c>
       <c r="C49">
-        <v>900</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2">
-        <v>44274.38597222222</v>
+        <v>44293.38597222222</v>
       </c>
       <c r="B50">
-        <v>14502.5</v>
+        <v>14742.2998046875</v>
       </c>
       <c r="C50">
-        <v>2175</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2">
-        <v>44274.3859837963</v>
+        <v>44293.3859837963</v>
       </c>
       <c r="B51">
-        <v>14500</v>
+        <v>14739.099609375</v>
       </c>
       <c r="C51">
-        <v>1275</v>
+        <v>7650</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2">
-        <v>44274.38599537037</v>
+        <v>44293.38599537037</v>
       </c>
       <c r="B52">
-        <v>14499.7998046875</v>
+        <v>14742.599609375</v>
       </c>
       <c r="C52">
-        <v>825</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2">
-        <v>44274.38600694444</v>
+        <v>44293.38600694444</v>
       </c>
       <c r="B53">
-        <v>14498.150390625</v>
+        <v>14744.349609375</v>
       </c>
       <c r="C53">
-        <v>1275</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2">
-        <v>44274.38601851852</v>
+        <v>44293.38601851852</v>
       </c>
       <c r="B54">
-        <v>14499.5</v>
+        <v>14743.7998046875</v>
       </c>
       <c r="C54">
-        <v>1200</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2">
-        <v>44274.3860300926</v>
+        <v>44293.3860300926</v>
       </c>
       <c r="B55">
-        <v>14498.75</v>
+        <v>14745.75</v>
       </c>
       <c r="C55">
-        <v>1275</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2">
-        <v>44274.38604166666</v>
+        <v>44293.38604166666</v>
       </c>
       <c r="B56">
-        <v>14498.099609375</v>
+        <v>14748.400390625</v>
       </c>
       <c r="C56">
-        <v>1275</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2">
-        <v>44274.38605324074</v>
+        <v>44293.38605324074</v>
       </c>
       <c r="B57">
-        <v>14499</v>
+        <v>14754.7998046875</v>
       </c>
       <c r="C57">
-        <v>2025</v>
+        <v>13800</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2">
-        <v>44274.38606481482</v>
+        <v>44293.38606481482</v>
       </c>
       <c r="B58">
-        <v>14495</v>
+        <v>14757.2998046875</v>
       </c>
       <c r="C58">
-        <v>3150</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2">
-        <v>44274.38607638889</v>
+        <v>44293.38607638889</v>
       </c>
       <c r="B59">
-        <v>14496.849609375</v>
+        <v>14759.5</v>
       </c>
       <c r="C59">
-        <v>2250</v>
+        <v>18375</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2">
-        <v>44274.38608796296</v>
+        <v>44293.38608796296</v>
       </c>
       <c r="B60">
-        <v>14495.75</v>
+        <v>14761.0498046875</v>
       </c>
       <c r="C60">
-        <v>1275</v>
+        <v>4725</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2">
-        <v>44274.38609953703</v>
+        <v>44293.38609953703</v>
       </c>
       <c r="B61">
-        <v>14492</v>
+        <v>14761.099609375</v>
       </c>
       <c r="C61">
-        <v>4200</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2">
-        <v>44274.38611111111</v>
+        <v>44293.38611111111</v>
       </c>
       <c r="B62">
-        <v>14491.900390625</v>
+        <v>14755.650390625</v>
       </c>
       <c r="C62">
-        <v>900</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2">
-        <v>44274.38612268519</v>
+        <v>44293.38612268519</v>
       </c>
       <c r="B63">
-        <v>14490</v>
+        <v>14755.650390625</v>
       </c>
       <c r="C63">
-        <v>5475</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="2">
-        <v>44274.38613425926</v>
+        <v>44293.38613425926</v>
       </c>
       <c r="B64">
-        <v>14489.099609375</v>
+        <v>14759.5498046875</v>
       </c>
       <c r="C64">
-        <v>1575</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="2">
-        <v>44274.38614583333</v>
+        <v>44293.38614583333</v>
       </c>
       <c r="B65">
-        <v>14491.849609375</v>
+        <v>14762.25</v>
       </c>
       <c r="C65">
-        <v>4575</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="2">
-        <v>44274.38615740741</v>
+        <v>44293.38615740741</v>
       </c>
       <c r="B66">
-        <v>14493.9501953125</v>
+        <v>14757.349609375</v>
       </c>
       <c r="C66">
-        <v>4275</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2">
-        <v>44274.38616898148</v>
+        <v>44293.38616898148</v>
       </c>
       <c r="B67">
-        <v>14495</v>
+        <v>14755.4501953125</v>
       </c>
       <c r="C67">
-        <v>4575</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="2">
-        <v>44274.38618055556</v>
+        <v>44293.38618055556</v>
       </c>
       <c r="B68">
-        <v>14497.5</v>
+        <v>14752.7001953125</v>
       </c>
       <c r="C68">
-        <v>1650</v>
+        <v>975</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="2">
-        <v>44274.38619212963</v>
+        <v>44293.38619212963</v>
       </c>
       <c r="B69">
-        <v>14499.2001953125</v>
+        <v>14753</v>
       </c>
       <c r="C69">
-        <v>1650</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="2">
-        <v>44274.3862037037</v>
+        <v>44293.3862037037</v>
       </c>
       <c r="B70">
-        <v>14497.5</v>
+        <v>14750</v>
       </c>
       <c r="C70">
-        <v>825</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="2">
-        <v>44274.38621527778</v>
+        <v>44293.38621527778</v>
       </c>
       <c r="B71">
-        <v>14499.4501953125</v>
+        <v>14750</v>
       </c>
       <c r="C71">
-        <v>1350</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="2">
-        <v>44274.38622685185</v>
+        <v>44293.38622685185</v>
       </c>
       <c r="B72">
-        <v>14499.9501953125</v>
+        <v>14745.5</v>
       </c>
       <c r="C72">
-        <v>900</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="2">
-        <v>44274.38623842593</v>
+        <v>44293.38623842593</v>
       </c>
       <c r="B73">
-        <v>14501.4501953125</v>
+        <v>14740.349609375</v>
       </c>
       <c r="C73">
-        <v>3975</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="2">
-        <v>44274.38625</v>
+        <v>44293.38625</v>
       </c>
       <c r="B74">
-        <v>14502.5498046875</v>
+        <v>14745.5498046875</v>
       </c>
       <c r="C74">
-        <v>1125</v>
+        <v>6300</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="2">
-        <v>44274.38626157407</v>
+        <v>44293.38626157407</v>
       </c>
       <c r="B75">
-        <v>14502.75</v>
+        <v>14744.5</v>
       </c>
       <c r="C75">
-        <v>975</v>
+        <v>300</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="2">
-        <v>44274.38627314815</v>
+        <v>44293.38627314815</v>
       </c>
       <c r="B76">
-        <v>14504.900390625</v>
+        <v>14746.0498046875</v>
       </c>
       <c r="C76">
-        <v>750</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="2">
-        <v>44274.38628472222</v>
+        <v>44293.38628472222</v>
       </c>
       <c r="B77">
-        <v>14505.2998046875</v>
+        <v>14752</v>
       </c>
       <c r="C77">
-        <v>2700</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="2">
-        <v>44274.3862962963</v>
+        <v>44293.3862962963</v>
       </c>
       <c r="B78">
-        <v>14507.849609375</v>
+        <v>14750.7998046875</v>
       </c>
       <c r="C78">
-        <v>2400</v>
+        <v>675</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="2">
-        <v>44274.38630787037</v>
+        <v>44293.38630787037</v>
       </c>
       <c r="B79">
-        <v>14507.7001953125</v>
+        <v>14751.4501953125</v>
       </c>
       <c r="C79">
-        <v>1650</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="2">
-        <v>44274.38631944444</v>
+        <v>44293.38631944444</v>
       </c>
       <c r="B80">
-        <v>14506.5</v>
+        <v>14754.7001953125</v>
       </c>
       <c r="C80">
-        <v>1125</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="2">
-        <v>44274.38633101852</v>
+        <v>44293.38633101852</v>
       </c>
       <c r="B81">
-        <v>14505.7001953125</v>
+        <v>14749</v>
       </c>
       <c r="C81">
-        <v>450</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="2">
-        <v>44274.3863425926</v>
+        <v>44293.3863425926</v>
       </c>
       <c r="B82">
-        <v>14505.9501953125</v>
+        <v>14752.349609375</v>
       </c>
       <c r="C82">
-        <v>1125</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="2">
-        <v>44274.38635416667</v>
+        <v>44293.38635416667</v>
       </c>
       <c r="B83">
-        <v>14505</v>
+        <v>14749.5</v>
       </c>
       <c r="C83">
-        <v>1275</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="2">
-        <v>44274.38636574074</v>
+        <v>44293.38636574074</v>
       </c>
       <c r="B84">
-        <v>14506.150390625</v>
+        <v>14750.75</v>
       </c>
       <c r="C84">
-        <v>1950</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="2">
-        <v>44274.38637731481</v>
+        <v>44293.38637731481</v>
       </c>
       <c r="B85">
-        <v>14509</v>
+        <v>14754.7001953125</v>
       </c>
       <c r="C85">
-        <v>1200</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="2">
-        <v>44274.38638888889</v>
+        <v>44293.38638888889</v>
       </c>
       <c r="B86">
-        <v>14509.2998046875</v>
+        <v>14757.5</v>
       </c>
       <c r="C86">
-        <v>675</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="2">
-        <v>44274.38640046296</v>
+        <v>44293.38640046296</v>
       </c>
       <c r="B87">
-        <v>14508.400390625</v>
+        <v>14751.650390625</v>
       </c>
       <c r="C87">
-        <v>6900</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="2">
-        <v>44274.38641203703</v>
+        <v>44293.38641203703</v>
       </c>
       <c r="B88">
-        <v>14509.5498046875</v>
+        <v>14754.2001953125</v>
       </c>
       <c r="C88">
-        <v>1875</v>
+        <v>825</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="2">
-        <v>44274.38642361111</v>
+        <v>44293.38642361111</v>
       </c>
       <c r="B89">
-        <v>14506.75</v>
+        <v>14750.900390625</v>
       </c>
       <c r="C89">
-        <v>600</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="2">
-        <v>44274.38643518519</v>
+        <v>44293.38643518519</v>
       </c>
       <c r="B90">
-        <v>14509</v>
+        <v>14758.099609375</v>
       </c>
       <c r="C90">
-        <v>2250</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="2">
-        <v>44274.38644675926</v>
+        <v>44293.38644675926</v>
       </c>
       <c r="B91">
-        <v>14507.25</v>
+        <v>14755</v>
       </c>
       <c r="C91">
-        <v>675</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="2">
-        <v>44274.38645833333</v>
+        <v>44293.38645833333</v>
       </c>
       <c r="B92">
-        <v>14507.099609375</v>
+        <v>14757.2001953125</v>
       </c>
       <c r="C92">
         <v>375</v>
@@ -1404,824 +1404,835 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="2">
-        <v>44274.3864699074</v>
+        <v>44293.3864699074</v>
       </c>
       <c r="B93">
-        <v>14507</v>
+        <v>14756.5498046875</v>
       </c>
       <c r="C93">
-        <v>150</v>
+        <v>825</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="2">
-        <v>44274.38648148148</v>
+        <v>44293.38648148148</v>
       </c>
       <c r="B94">
-        <v>14505.25</v>
+        <v>14757.0498046875</v>
       </c>
       <c r="C94">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="2">
-        <v>44274.38649305556</v>
-      </c>
-      <c r="B95">
-        <v>14505.9501953125</v>
-      </c>
-      <c r="C95">
-        <v>1125</v>
+        <v>675</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="2">
-        <v>44274.38650462963</v>
+        <v>44293.38650462963</v>
       </c>
       <c r="B96">
-        <v>14504.5</v>
+        <v>14758.150390625</v>
       </c>
       <c r="C96">
-        <v>1275</v>
+        <v>600</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="2">
-        <v>44274.3865162037</v>
+        <v>44293.3865162037</v>
       </c>
       <c r="B97">
-        <v>14503.2001953125</v>
+        <v>14762.9501953125</v>
       </c>
       <c r="C97">
-        <v>675</v>
+        <v>9375</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="2">
-        <v>44274.38652777778</v>
+        <v>44293.38652777778</v>
       </c>
       <c r="B98">
-        <v>14502.7998046875</v>
+        <v>14764</v>
       </c>
       <c r="C98">
-        <v>225</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="2">
-        <v>44274.38653935185</v>
+        <v>44293.38653935185</v>
       </c>
       <c r="B99">
-        <v>14502.150390625</v>
+        <v>14764.150390625</v>
       </c>
       <c r="C99">
-        <v>1200</v>
+        <v>3450</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="2">
-        <v>44274.38655092593</v>
+        <v>44293.38655092593</v>
       </c>
       <c r="B100">
-        <v>14504.900390625</v>
+        <v>14764</v>
       </c>
       <c r="C100">
-        <v>600</v>
+        <v>525</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="2">
-        <v>44274.3865625</v>
+        <v>44293.3865625</v>
       </c>
       <c r="B101">
-        <v>14504.349609375</v>
+        <v>14762</v>
       </c>
       <c r="C101">
-        <v>1275</v>
+        <v>300</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="2">
-        <v>44274.38657407407</v>
+        <v>44293.38657407407</v>
       </c>
       <c r="B102">
-        <v>14505</v>
+        <v>14763.2998046875</v>
       </c>
       <c r="C102">
-        <v>10425</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="2">
-        <v>44274.38658564815</v>
+        <v>44293.38658564815</v>
       </c>
       <c r="B103">
-        <v>14504.0498046875</v>
+        <v>14760.9501953125</v>
       </c>
       <c r="C103">
-        <v>1350</v>
+        <v>17700</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="2">
-        <v>44274.38659722222</v>
+        <v>44293.38659722222</v>
       </c>
       <c r="B104">
-        <v>14503.9501953125</v>
+        <v>14765</v>
       </c>
       <c r="C104">
-        <v>750</v>
+        <v>5925</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="2">
-        <v>44274.3866087963</v>
+        <v>44293.3866087963</v>
       </c>
       <c r="B105">
-        <v>14502.0498046875</v>
+        <v>14766.4501953125</v>
       </c>
       <c r="C105">
-        <v>1650</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="2">
-        <v>44274.38662037037</v>
+        <v>44293.38662037037</v>
       </c>
       <c r="B106">
-        <v>14503.5</v>
+        <v>14763.5</v>
       </c>
       <c r="C106">
-        <v>975</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="2">
-        <v>44274.38663194444</v>
+        <v>44293.38663194444</v>
       </c>
       <c r="B107">
-        <v>14502.75</v>
+        <v>14771.7998046875</v>
       </c>
       <c r="C107">
-        <v>825</v>
+        <v>11850</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="2">
-        <v>44274.38664351852</v>
+        <v>44293.38664351852</v>
       </c>
       <c r="B108">
-        <v>14501</v>
+        <v>14761</v>
       </c>
       <c r="C108">
-        <v>1275</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="2">
-        <v>44274.3866550926</v>
+        <v>44293.3866550926</v>
       </c>
       <c r="B109">
-        <v>14501.7998046875</v>
+        <v>14760</v>
       </c>
       <c r="C109">
-        <v>750</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="2">
-        <v>44274.38666666667</v>
+        <v>44293.38666666667</v>
       </c>
       <c r="B110">
-        <v>14499.2001953125</v>
+        <v>14762.7001953125</v>
       </c>
       <c r="C110">
-        <v>6075</v>
+        <v>825</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="2">
-        <v>44274.38667824074</v>
+        <v>44293.38667824074</v>
       </c>
       <c r="B111">
-        <v>14499.25</v>
+        <v>14764</v>
       </c>
       <c r="C111">
-        <v>1350</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="2">
-        <v>44274.38668981481</v>
+        <v>44293.38668981481</v>
       </c>
       <c r="B112">
-        <v>14496.9501953125</v>
+        <v>14765.25</v>
       </c>
       <c r="C112">
-        <v>1500</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="2">
-        <v>44274.38670138889</v>
+        <v>44293.38670138889</v>
       </c>
       <c r="B113">
-        <v>14494.25</v>
+        <v>14766.25</v>
       </c>
       <c r="C113">
-        <v>1125</v>
+        <v>825</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="2">
-        <v>44274.38671296297</v>
+        <v>44293.38671296297</v>
       </c>
       <c r="B114">
-        <v>14492.900390625</v>
+        <v>14767.599609375</v>
       </c>
       <c r="C114">
-        <v>900</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="2">
-        <v>44274.38672453703</v>
+        <v>44293.38672453703</v>
       </c>
       <c r="B115">
-        <v>14490.099609375</v>
+        <v>14766.5</v>
       </c>
       <c r="C115">
-        <v>900</v>
+        <v>525</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="2">
-        <v>44274.38673611111</v>
+        <v>44293.38673611111</v>
       </c>
       <c r="B116">
-        <v>14492.7001953125</v>
+        <v>14763.25</v>
       </c>
       <c r="C116">
-        <v>2550</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="2">
-        <v>44274.38674768519</v>
+        <v>44293.38674768519</v>
       </c>
       <c r="B117">
-        <v>14490.5</v>
+        <v>14766.25</v>
       </c>
       <c r="C117">
-        <v>1800</v>
+        <v>150</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="2">
-        <v>44274.38675925926</v>
+        <v>44293.38675925926</v>
       </c>
       <c r="B118">
-        <v>14489.150390625</v>
+        <v>14765</v>
       </c>
       <c r="C118">
-        <v>2100</v>
+        <v>525</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="2">
-        <v>44274.38677083333</v>
+        <v>44293.38677083333</v>
       </c>
       <c r="B119">
-        <v>14489.099609375</v>
+        <v>14765</v>
       </c>
       <c r="C119">
-        <v>2700</v>
+        <v>225</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="2">
-        <v>44274.3867824074</v>
+        <v>44293.3867824074</v>
       </c>
       <c r="B120">
-        <v>14489.099609375</v>
+        <v>14762</v>
       </c>
       <c r="C120">
-        <v>3450</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="2">
-        <v>44274.38679398148</v>
+        <v>44293.38679398148</v>
       </c>
       <c r="B121">
-        <v>14489.099609375</v>
+        <v>14759.5</v>
       </c>
       <c r="C121">
-        <v>3300</v>
+        <v>225</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="2">
-        <v>44274.38680555556</v>
+        <v>44293.38680555556</v>
       </c>
       <c r="B122">
-        <v>14489.099609375</v>
+        <v>14760.0498046875</v>
       </c>
       <c r="C122">
-        <v>2775</v>
+        <v>450</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="2">
-        <v>44274.38681712963</v>
+        <v>44293.38681712963</v>
       </c>
       <c r="B123">
-        <v>14489.099609375</v>
+        <v>14763.4501953125</v>
       </c>
       <c r="C123">
-        <v>9150</v>
+        <v>600</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="2">
-        <v>44274.3868287037</v>
+        <v>44293.3868287037</v>
       </c>
       <c r="B124">
-        <v>14488.25</v>
+        <v>14759.9501953125</v>
       </c>
       <c r="C124">
-        <v>8475</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="2">
-        <v>44274.38684027778</v>
+        <v>44293.38684027778</v>
       </c>
       <c r="B125">
-        <v>14487.25</v>
+        <v>14757.25</v>
       </c>
       <c r="C125">
-        <v>2325</v>
+        <v>75</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="2">
-        <v>44274.38685185185</v>
+        <v>44293.38685185185</v>
       </c>
       <c r="B126">
-        <v>14483.2998046875</v>
+        <v>14761.849609375</v>
       </c>
       <c r="C126">
-        <v>3375</v>
+        <v>600</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="2">
-        <v>44274.38686342593</v>
+        <v>44293.38686342593</v>
       </c>
       <c r="B127">
-        <v>14483</v>
+        <v>14758.5</v>
       </c>
       <c r="C127">
-        <v>3675</v>
+        <v>900</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="2">
-        <v>44274.386875</v>
+        <v>44293.386875</v>
       </c>
       <c r="B128">
-        <v>14483</v>
+        <v>14759.4501953125</v>
       </c>
       <c r="C128">
-        <v>1800</v>
+        <v>525</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="2">
-        <v>44274.38688657407</v>
+        <v>44293.38688657407</v>
       </c>
       <c r="B129">
-        <v>14482.849609375</v>
+        <v>14760.849609375</v>
       </c>
       <c r="C129">
-        <v>1350</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="2">
-        <v>44274.38689814815</v>
+        <v>44293.38689814815</v>
       </c>
       <c r="B130">
-        <v>14482.2001953125</v>
+        <v>14761.849609375</v>
       </c>
       <c r="C130">
-        <v>1425</v>
+        <v>375</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="2">
-        <v>44274.38690972222</v>
+        <v>44293.38690972222</v>
       </c>
       <c r="B131">
-        <v>14482.2001953125</v>
+        <v>14760.5</v>
       </c>
       <c r="C131">
-        <v>1050</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="2">
-        <v>44274.3869212963</v>
+        <v>44293.3869212963</v>
       </c>
       <c r="B132">
-        <v>14482.2001953125</v>
+        <v>14762.75</v>
       </c>
       <c r="C132">
-        <v>3300</v>
+        <v>300</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="2">
-        <v>44274.38693287037</v>
+        <v>44293.38693287037</v>
       </c>
       <c r="B133">
-        <v>14482.150390625</v>
+        <v>14763</v>
       </c>
       <c r="C133">
-        <v>750</v>
+        <v>900</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="2">
-        <v>44274.38694444444</v>
+        <v>44293.38694444444</v>
       </c>
       <c r="B134">
-        <v>14482</v>
+        <v>14765</v>
       </c>
       <c r="C134">
-        <v>3225</v>
+        <v>375</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="2">
-        <v>44274.38695601852</v>
+        <v>44293.38695601852</v>
       </c>
       <c r="B135">
-        <v>14482.349609375</v>
+        <v>14767.5</v>
       </c>
       <c r="C135">
-        <v>375</v>
+        <v>975</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="2">
-        <v>44274.3869675926</v>
+        <v>44293.3869675926</v>
       </c>
       <c r="B136">
-        <v>14482.400390625</v>
+        <v>14766.75</v>
       </c>
       <c r="C136">
-        <v>975</v>
+        <v>300</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2">
-        <v>44274.38697916667</v>
+        <v>44293.38697916667</v>
       </c>
       <c r="B137">
-        <v>14481.2001953125</v>
+        <v>14769</v>
       </c>
       <c r="C137">
-        <v>2175</v>
+        <v>450</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="2">
-        <v>44274.38699074074</v>
+        <v>44293.38699074074</v>
       </c>
       <c r="B138">
-        <v>14480.2001953125</v>
+        <v>14767.5498046875</v>
       </c>
       <c r="C138">
-        <v>1800</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="2">
-        <v>44274.38700231481</v>
+        <v>44293.38700231481</v>
       </c>
       <c r="B139">
-        <v>14482</v>
+        <v>14767</v>
       </c>
       <c r="C139">
-        <v>525</v>
+        <v>6450</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="2">
-        <v>44274.38701388889</v>
+        <v>44293.38701388889</v>
       </c>
       <c r="B140">
-        <v>14482</v>
+        <v>14769.2001953125</v>
       </c>
       <c r="C140">
-        <v>525</v>
+        <v>750</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="2">
-        <v>44274.38702546297</v>
+        <v>44293.38702546297</v>
       </c>
       <c r="B141">
-        <v>14482.7001953125</v>
+        <v>14767</v>
       </c>
       <c r="C141">
-        <v>1425</v>
+        <v>375</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="2">
-        <v>44274.38703703704</v>
+        <v>44293.38703703704</v>
       </c>
       <c r="B142">
-        <v>14482.099609375</v>
+        <v>14772.2001953125</v>
       </c>
       <c r="C142">
-        <v>1050</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="2">
-        <v>44274.38704861111</v>
+        <v>44293.38704861111</v>
       </c>
       <c r="B143">
-        <v>14482.849609375</v>
+        <v>14774.2998046875</v>
       </c>
       <c r="C143">
-        <v>2250</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="2">
-        <v>44274.38706018519</v>
+        <v>44293.38706018519</v>
       </c>
       <c r="B144">
-        <v>14482</v>
+        <v>14770.4501953125</v>
       </c>
       <c r="C144">
-        <v>600</v>
+        <v>375</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="2">
-        <v>44274.38707175926</v>
+        <v>44293.38707175926</v>
       </c>
       <c r="B145">
-        <v>14482.7998046875</v>
+        <v>14772.2998046875</v>
       </c>
       <c r="C145">
-        <v>525</v>
+        <v>225</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="2">
-        <v>44274.38708333333</v>
+        <v>44293.38708333333</v>
       </c>
       <c r="B146">
-        <v>14482.099609375</v>
+        <v>14776.5</v>
       </c>
       <c r="C146">
-        <v>675</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="2">
-        <v>44274.3870949074</v>
+        <v>44293.3870949074</v>
       </c>
       <c r="B147">
-        <v>14481.5498046875</v>
+        <v>14773.349609375</v>
       </c>
       <c r="C147">
-        <v>525</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="2">
-        <v>44274.38710648148</v>
+        <v>44293.38710648148</v>
       </c>
       <c r="B148">
-        <v>14480.150390625</v>
+        <v>14778</v>
       </c>
       <c r="C148">
-        <v>975</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="2">
-        <v>44274.38711805556</v>
+        <v>44293.38711805556</v>
       </c>
       <c r="B149">
-        <v>14480.150390625</v>
+        <v>14779.75</v>
       </c>
       <c r="C149">
-        <v>675</v>
+        <v>5850</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="2">
-        <v>44274.38712962963</v>
+        <v>44293.38712962963</v>
       </c>
       <c r="B150">
-        <v>14481</v>
+        <v>14778.150390625</v>
       </c>
       <c r="C150">
-        <v>975</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="2">
-        <v>44274.3871412037</v>
+        <v>44293.3871412037</v>
       </c>
       <c r="B151">
-        <v>14481.599609375</v>
+        <v>14780</v>
       </c>
       <c r="C151">
-        <v>675</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="2">
-        <v>44274.38715277778</v>
+        <v>44293.38715277778</v>
       </c>
       <c r="B152">
-        <v>14480.2001953125</v>
+        <v>14781.5498046875</v>
       </c>
       <c r="C152">
-        <v>1275</v>
+        <v>825</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="2">
-        <v>44274.38716435185</v>
+        <v>44293.38716435185</v>
       </c>
       <c r="B153">
-        <v>14480</v>
+        <v>14783.099609375</v>
       </c>
       <c r="C153">
-        <v>2400</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="2">
-        <v>44274.38717592593</v>
+        <v>44293.38717592593</v>
       </c>
       <c r="B154">
-        <v>14480</v>
+        <v>14785</v>
       </c>
       <c r="C154">
-        <v>600</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="2">
-        <v>44274.3871875</v>
+        <v>44293.3871875</v>
       </c>
       <c r="B155">
-        <v>14480</v>
+        <v>14787.5</v>
       </c>
       <c r="C155">
-        <v>2475</v>
+        <v>5475</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="2">
-        <v>44274.38719907407</v>
+        <v>44293.38719907407</v>
       </c>
       <c r="B156">
-        <v>14480</v>
+        <v>14779.849609375</v>
       </c>
       <c r="C156">
-        <v>4425</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="2">
-        <v>44274.38721064815</v>
+        <v>44293.38721064815</v>
       </c>
       <c r="B157">
-        <v>14477.099609375</v>
+        <v>14779.650390625</v>
       </c>
       <c r="C157">
-        <v>1650</v>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="2">
+        <v>44293.38722222222</v>
+      </c>
+      <c r="B158">
+        <v>14783.7998046875</v>
+      </c>
+      <c r="C158">
+        <v>750</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="2">
-        <v>44274.3872337963</v>
+        <v>44293.3872337963</v>
       </c>
       <c r="B159">
-        <v>14476.7998046875</v>
+        <v>14780.400390625</v>
       </c>
       <c r="C159">
-        <v>1575</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="2">
-        <v>44274.38724537037</v>
+        <v>44293.38724537037</v>
       </c>
       <c r="B160">
-        <v>14476.4501953125</v>
+        <v>14773.2001953125</v>
       </c>
       <c r="C160">
-        <v>675</v>
+        <v>5250</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="2">
-        <v>44274.38725694444</v>
+        <v>44293.38725694444</v>
       </c>
       <c r="B161">
-        <v>14477</v>
+        <v>14778.25</v>
       </c>
       <c r="C161">
-        <v>675</v>
+        <v>600</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="2">
-        <v>44274.38726851852</v>
+        <v>44293.38726851852</v>
       </c>
       <c r="B162">
-        <v>14476.599609375</v>
+        <v>14782.150390625</v>
       </c>
       <c r="C162">
-        <v>1200</v>
+        <v>450</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="2">
-        <v>44274.38728009259</v>
+        <v>44293.38728009259</v>
       </c>
       <c r="B163">
-        <v>14477.0498046875</v>
+        <v>14781.25</v>
       </c>
       <c r="C163">
-        <v>2550</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="2">
+        <v>44293.38729166667</v>
+      </c>
+      <c r="B164">
+        <v>14776.7998046875</v>
+      </c>
+      <c r="C164">
+        <v>1350</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="2">
-        <v>44274.38730324074</v>
+        <v>44293.38730324074</v>
       </c>
       <c r="B165">
-        <v>14476.125</v>
+        <v>14777.150390625</v>
       </c>
       <c r="C165">
-        <v>2250</v>
+        <v>750</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="2">
-        <v>44274.38731481481</v>
+        <v>44293.38731481481</v>
       </c>
       <c r="B166">
-        <v>14477</v>
+        <v>14775.0498046875</v>
       </c>
       <c r="C166">
-        <v>1125</v>
+        <v>675</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="2">
-        <v>44274.38732638889</v>
+        <v>44293.38732638889</v>
       </c>
       <c r="B167">
-        <v>14476.150390625</v>
+        <v>14779.2001953125</v>
       </c>
       <c r="C167">
-        <v>525</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="2">
-        <v>44274.38733796297</v>
+        <v>44293.38733796297</v>
       </c>
       <c r="B168">
-        <v>14477.900390625</v>
+        <v>14776.400390625</v>
       </c>
       <c r="C168">
-        <v>1350</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="2">
-        <v>44274.38734953704</v>
+        <v>44293.38734953704</v>
       </c>
       <c r="B169">
-        <v>14476.150390625</v>
+        <v>14773.25</v>
       </c>
       <c r="C169">
         <v>675</v>
@@ -2229,1333 +2240,1421 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="2">
-        <v>44274.38736111111</v>
+        <v>44293.38736111111</v>
       </c>
       <c r="B170">
-        <v>14477</v>
+        <v>14772</v>
       </c>
       <c r="C170">
-        <v>300</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="2">
-        <v>44274.38737268518</v>
+        <v>44293.38737268518</v>
       </c>
       <c r="B171">
-        <v>14477</v>
+        <v>14774.5</v>
       </c>
       <c r="C171">
-        <v>2025</v>
+        <v>450</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="2">
-        <v>44274.38738425926</v>
+        <v>44293.38738425926</v>
       </c>
       <c r="B172">
-        <v>14477</v>
+        <v>14771</v>
       </c>
       <c r="C172">
-        <v>1950</v>
+        <v>975</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="2">
-        <v>44274.38739583334</v>
+        <v>44293.38739583334</v>
       </c>
       <c r="B173">
-        <v>14477</v>
+        <v>14769.75</v>
       </c>
       <c r="C173">
-        <v>600</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="2">
-        <v>44274.3874074074</v>
+        <v>44293.3874074074</v>
       </c>
       <c r="B174">
-        <v>14476.099609375</v>
+        <v>14770.25</v>
       </c>
       <c r="C174">
-        <v>675</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="2">
-        <v>44274.38741898148</v>
+        <v>44293.38741898148</v>
       </c>
       <c r="B175">
-        <v>14476.150390625</v>
+        <v>14774.099609375</v>
       </c>
       <c r="C175">
-        <v>450</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="2">
-        <v>44274.38743055556</v>
+        <v>44293.38743055556</v>
       </c>
       <c r="B176">
-        <v>14475.2998046875</v>
+        <v>14778</v>
       </c>
       <c r="C176">
-        <v>3075</v>
+        <v>825</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="2">
-        <v>44274.38744212963</v>
+        <v>44293.38744212963</v>
       </c>
       <c r="B177">
-        <v>14473.599609375</v>
+        <v>14777.7998046875</v>
       </c>
       <c r="C177">
-        <v>6150</v>
+        <v>900</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="2">
-        <v>44274.3874537037</v>
+        <v>44293.3874537037</v>
       </c>
       <c r="B178">
-        <v>14473</v>
+        <v>14778</v>
       </c>
       <c r="C178">
-        <v>2100</v>
+        <v>675</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="2">
-        <v>44274.38747685185</v>
+        <v>44293.38747685185</v>
       </c>
       <c r="B180">
-        <v>14472</v>
+        <v>14777.7998046875</v>
       </c>
       <c r="C180">
-        <v>3900</v>
+        <v>450</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="2">
-        <v>44274.38748842593</v>
+        <v>44293.38748842593</v>
       </c>
       <c r="B181">
-        <v>14472.5</v>
+        <v>14778</v>
       </c>
       <c r="C181">
-        <v>1275</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="2">
-        <v>44274.3875</v>
+        <v>44293.3875</v>
       </c>
       <c r="B182">
-        <v>14471.85009765625</v>
+        <v>14779.400390625</v>
       </c>
       <c r="C182">
-        <v>2475</v>
+        <v>900</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="2">
-        <v>44274.38751157407</v>
+        <v>44293.38751157407</v>
       </c>
       <c r="B183">
-        <v>14473.2001953125</v>
+        <v>14778.9501953125</v>
       </c>
       <c r="C183">
-        <v>1425</v>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="2">
+        <v>44293.38752314815</v>
+      </c>
+      <c r="B184">
+        <v>14776.400390625</v>
+      </c>
+      <c r="C184">
+        <v>1575</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="2">
-        <v>44274.38753472222</v>
+        <v>44293.38753472222</v>
       </c>
       <c r="B185">
-        <v>14470.52490234375</v>
+        <v>14776.2001953125</v>
       </c>
       <c r="C185">
-        <v>5400</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="2">
-        <v>44274.3875462963</v>
+        <v>44293.3875462963</v>
       </c>
       <c r="B186">
-        <v>14469.400390625</v>
+        <v>14779</v>
       </c>
       <c r="C186">
-        <v>4875</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="2">
-        <v>44274.38755787037</v>
+        <v>44293.38755787037</v>
       </c>
       <c r="B187">
-        <v>14468.599609375</v>
+        <v>14775.5498046875</v>
       </c>
       <c r="C187">
-        <v>600</v>
+        <v>975</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="2">
-        <v>44274.38756944444</v>
+        <v>44293.38756944444</v>
       </c>
       <c r="B188">
-        <v>14467.7998046875</v>
+        <v>14780</v>
       </c>
       <c r="C188">
-        <v>1350</v>
+        <v>975</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="2">
-        <v>44274.38758101852</v>
+        <v>44293.38758101852</v>
       </c>
       <c r="B189">
-        <v>14467</v>
+        <v>14778.9501953125</v>
       </c>
       <c r="C189">
-        <v>825</v>
+        <v>2775</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="2">
-        <v>44274.38759259259</v>
+        <v>44293.38759259259</v>
       </c>
       <c r="B190">
-        <v>14468.599609375</v>
+        <v>14776.599609375</v>
       </c>
       <c r="C190">
-        <v>4350</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="2">
-        <v>44274.38760416667</v>
+        <v>44293.38760416667</v>
       </c>
       <c r="B191">
-        <v>14469.0498046875</v>
+        <v>14776.599609375</v>
       </c>
       <c r="C191">
-        <v>1200</v>
+        <v>75</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="2">
-        <v>44274.38761574074</v>
+        <v>44293.38761574074</v>
       </c>
       <c r="B192">
-        <v>14468</v>
+        <v>14779</v>
       </c>
       <c r="C192">
-        <v>1650</v>
+        <v>975</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="2">
+        <v>44293.38762731481</v>
+      </c>
+      <c r="B193">
+        <v>14781.25</v>
+      </c>
+      <c r="C193">
+        <v>3750</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="2">
-        <v>44274.38763888889</v>
+        <v>44293.38763888889</v>
       </c>
       <c r="B194">
-        <v>14468.1748046875</v>
+        <v>14782.7001953125</v>
       </c>
       <c r="C194">
-        <v>1425</v>
+        <v>375</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="2">
-        <v>44274.38765046297</v>
+        <v>44293.38765046297</v>
       </c>
       <c r="B195">
-        <v>14468.7001953125</v>
+        <v>14783</v>
       </c>
       <c r="C195">
-        <v>1200</v>
+        <v>375</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="2">
-        <v>44274.38766203704</v>
+        <v>44293.38766203704</v>
       </c>
       <c r="B196">
-        <v>14468</v>
+        <v>14780</v>
       </c>
       <c r="C196">
-        <v>1800</v>
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="2">
+        <v>44293.38767361111</v>
+      </c>
+      <c r="B197">
+        <v>14781</v>
+      </c>
+      <c r="C197">
+        <v>1275</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="2">
-        <v>44274.38768518518</v>
+        <v>44293.38768518518</v>
       </c>
       <c r="B198">
-        <v>14465.7998046875</v>
+        <v>14780.5</v>
       </c>
       <c r="C198">
-        <v>5400</v>
+        <v>675</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="2">
+        <v>44293.38769675926</v>
+      </c>
+      <c r="B199">
+        <v>14777.5498046875</v>
+      </c>
+      <c r="C199">
+        <v>150</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="2">
-        <v>44274.38770833334</v>
+        <v>44293.38770833334</v>
       </c>
       <c r="B200">
-        <v>14465</v>
+        <v>14781.7998046875</v>
       </c>
       <c r="C200">
-        <v>4275</v>
+        <v>825</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="2">
-        <v>44274.3877199074</v>
+        <v>44293.3877199074</v>
       </c>
       <c r="B201">
-        <v>14466.099609375</v>
+        <v>14781.5</v>
       </c>
       <c r="C201">
-        <v>2850</v>
+        <v>825</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="2">
-        <v>44274.38773148148</v>
+        <v>44293.38773148148</v>
       </c>
       <c r="B202">
-        <v>14464.599609375</v>
+        <v>14780.5</v>
       </c>
       <c r="C202">
-        <v>5250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="2">
-        <v>44274.38774305556</v>
+        <v>44293.38774305556</v>
       </c>
       <c r="B203">
-        <v>14464</v>
+        <v>14778.5498046875</v>
       </c>
       <c r="C203">
-        <v>2400</v>
+        <v>900</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="2">
-        <v>44274.38775462963</v>
+        <v>44293.38775462963</v>
       </c>
       <c r="B204">
-        <v>14463</v>
+        <v>14776.25</v>
       </c>
       <c r="C204">
-        <v>1575</v>
+        <v>300</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="2">
-        <v>44274.3877662037</v>
+        <v>44293.3877662037</v>
       </c>
       <c r="B205">
-        <v>14462</v>
+        <v>14777</v>
       </c>
       <c r="C205">
-        <v>2025</v>
+        <v>675</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="2">
-        <v>44274.38777777777</v>
+        <v>44293.38777777777</v>
       </c>
       <c r="B206">
-        <v>14461.2998046875</v>
+        <v>14780</v>
       </c>
       <c r="C206">
-        <v>4200</v>
+        <v>750</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="2">
-        <v>44274.38778935185</v>
+        <v>44293.38778935185</v>
       </c>
       <c r="B207">
-        <v>14462.0498046875</v>
+        <v>14780.5498046875</v>
       </c>
       <c r="C207">
-        <v>1950</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="2">
-        <v>44274.38780092593</v>
+        <v>44293.38780092593</v>
       </c>
       <c r="B208">
-        <v>14460.2998046875</v>
+        <v>14780.5</v>
       </c>
       <c r="C208">
-        <v>2250</v>
+        <v>825</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="2">
-        <v>44274.3878125</v>
+        <v>44293.3878125</v>
       </c>
       <c r="B209">
-        <v>14456.9501953125</v>
+        <v>14778.5498046875</v>
       </c>
       <c r="C209">
-        <v>6000</v>
+        <v>150</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="2">
-        <v>44274.38782407407</v>
+        <v>44293.38782407407</v>
       </c>
       <c r="B210">
-        <v>14457.349609375</v>
+        <v>14781.7998046875</v>
       </c>
       <c r="C210">
-        <v>1200</v>
+        <v>3900</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="2">
-        <v>44274.38783564815</v>
+        <v>44293.38783564815</v>
       </c>
       <c r="B211">
-        <v>14456.099609375</v>
+        <v>14779.349609375</v>
       </c>
       <c r="C211">
-        <v>1200</v>
+        <v>375</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="2">
-        <v>44274.38784722222</v>
+        <v>44293.38784722222</v>
       </c>
       <c r="B212">
-        <v>14455</v>
+        <v>14782.150390625</v>
       </c>
       <c r="C212">
-        <v>1950</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="2">
-        <v>44274.3878587963</v>
+        <v>44293.3878587963</v>
       </c>
       <c r="B213">
-        <v>14452.2998046875</v>
+        <v>14782.150390625</v>
       </c>
       <c r="C213">
-        <v>1950</v>
+        <v>300</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="2">
-        <v>44274.38787037037</v>
+        <v>44293.38787037037</v>
       </c>
       <c r="B214">
-        <v>14452.0498046875</v>
+        <v>14782.599609375</v>
       </c>
       <c r="C214">
-        <v>3300</v>
+        <v>75</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="2">
-        <v>44274.38788194444</v>
+        <v>44293.38788194444</v>
       </c>
       <c r="B215">
-        <v>14455</v>
+        <v>14780.099609375</v>
       </c>
       <c r="C215">
-        <v>1725</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="2">
-        <v>44274.38789351852</v>
+        <v>44293.38789351852</v>
       </c>
       <c r="B216">
-        <v>14453.7998046875</v>
+        <v>14782.2998046875</v>
       </c>
       <c r="C216">
-        <v>1725</v>
+        <v>150</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="2">
-        <v>44274.38790509259</v>
+        <v>44293.38790509259</v>
       </c>
       <c r="B217">
-        <v>14455.349609375</v>
+        <v>14779.150390625</v>
       </c>
       <c r="C217">
-        <v>2625</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="2">
-        <v>44274.38791666667</v>
+        <v>44293.38791666667</v>
       </c>
       <c r="B218">
-        <v>14454.7998046875</v>
+        <v>14781.849609375</v>
       </c>
       <c r="C218">
-        <v>2100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="2">
-        <v>44274.38792824074</v>
+        <v>44293.38792824074</v>
       </c>
       <c r="B219">
-        <v>14452.5498046875</v>
+        <v>14782</v>
       </c>
       <c r="C219">
-        <v>1425</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="2">
-        <v>44274.38793981481</v>
+        <v>44293.38793981481</v>
       </c>
       <c r="B220">
-        <v>14455</v>
+        <v>14781.400390625</v>
       </c>
       <c r="C220">
-        <v>3900</v>
+        <v>150</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="2">
-        <v>44274.38795138889</v>
+        <v>44293.38795138889</v>
       </c>
       <c r="B221">
-        <v>14455</v>
+        <v>14782</v>
       </c>
       <c r="C221">
-        <v>975</v>
+        <v>225</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="2">
-        <v>44274.38796296297</v>
+        <v>44293.38796296297</v>
       </c>
       <c r="B222">
-        <v>14457</v>
+        <v>14783.900390625</v>
       </c>
       <c r="C222">
-        <v>2775</v>
+        <v>375</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="2">
-        <v>44274.38797453704</v>
+        <v>44293.38797453704</v>
       </c>
       <c r="B223">
-        <v>14457.150390625</v>
+        <v>14783.0498046875</v>
       </c>
       <c r="C223">
-        <v>1050</v>
+        <v>150</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="2">
-        <v>44274.38798611111</v>
+        <v>44293.38798611111</v>
       </c>
       <c r="B224">
-        <v>14458.099609375</v>
+        <v>14780</v>
       </c>
       <c r="C224">
-        <v>2100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="2">
-        <v>44274.38799768518</v>
+        <v>44293.38799768518</v>
       </c>
       <c r="B225">
-        <v>14457.099609375</v>
+        <v>14780</v>
       </c>
       <c r="C225">
-        <v>675</v>
+        <v>450</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="2">
-        <v>44274.38800925926</v>
+        <v>44293.38800925926</v>
       </c>
       <c r="B226">
-        <v>14459.5</v>
+        <v>14781.5498046875</v>
       </c>
       <c r="C226">
-        <v>225</v>
+        <v>450</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="2">
-        <v>44274.38802083334</v>
+        <v>44293.38802083334</v>
       </c>
       <c r="B227">
-        <v>14459.5</v>
+        <v>14781.5</v>
       </c>
       <c r="C227">
-        <v>525</v>
+        <v>375</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="2">
-        <v>44274.38803240741</v>
+        <v>44293.38803240741</v>
       </c>
       <c r="B228">
-        <v>14457</v>
+        <v>14781.5</v>
       </c>
       <c r="C228">
-        <v>1350</v>
+        <v>150</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" s="2">
-        <v>44274.38804398148</v>
+        <v>44293.38804398148</v>
       </c>
       <c r="B229">
-        <v>14455</v>
+        <v>14779.349609375</v>
       </c>
       <c r="C229">
-        <v>1650</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="2">
-        <v>44274.38805555556</v>
+        <v>44293.38805555556</v>
       </c>
       <c r="B230">
-        <v>14458</v>
+        <v>14778.150390625</v>
       </c>
       <c r="C230">
-        <v>2025</v>
+        <v>525</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="2">
-        <v>44274.38806712963</v>
+        <v>44293.38806712963</v>
       </c>
       <c r="B231">
-        <v>14457.349609375</v>
+        <v>14783</v>
       </c>
       <c r="C231">
-        <v>750</v>
+        <v>675</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="2">
-        <v>44274.38807870371</v>
+        <v>44293.38807870371</v>
       </c>
       <c r="B232">
-        <v>14458.099609375</v>
+        <v>14784</v>
       </c>
       <c r="C232">
-        <v>1275</v>
+        <v>450</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="2">
-        <v>44274.38809027777</v>
+        <v>44293.38809027777</v>
       </c>
       <c r="B233">
-        <v>14458.4501953125</v>
+        <v>14783.4501953125</v>
       </c>
       <c r="C233">
-        <v>1650</v>
+        <v>600</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="2">
-        <v>44274.38810185185</v>
+        <v>44293.38810185185</v>
       </c>
       <c r="B234">
-        <v>14458.599609375</v>
+        <v>14781.4501953125</v>
       </c>
       <c r="C234">
-        <v>900</v>
+        <v>300</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="2">
-        <v>44274.38811342593</v>
+        <v>44293.38811342593</v>
       </c>
       <c r="B235">
-        <v>14458.599609375</v>
+        <v>14779</v>
       </c>
       <c r="C235">
-        <v>900</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="2">
-        <v>44274.388125</v>
+        <v>44293.388125</v>
       </c>
       <c r="B236">
-        <v>14458.599609375</v>
+        <v>14782.7998046875</v>
       </c>
       <c r="C236">
-        <v>1500</v>
+        <v>150</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="2">
-        <v>44274.38813657407</v>
+        <v>44293.38813657407</v>
       </c>
       <c r="B237">
-        <v>14458.099609375</v>
+        <v>14781.5</v>
       </c>
       <c r="C237">
-        <v>1425</v>
+        <v>75</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="2">
-        <v>44274.38814814815</v>
+        <v>44293.38814814815</v>
       </c>
       <c r="B238">
-        <v>14458</v>
+        <v>14779.5</v>
       </c>
       <c r="C238">
-        <v>1350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="2">
-        <v>44274.38815972222</v>
+        <v>44293.38815972222</v>
       </c>
       <c r="B239">
-        <v>14456.099609375</v>
+        <v>14781.25</v>
       </c>
       <c r="C239">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" s="2">
-        <v>44274.3881712963</v>
-      </c>
-      <c r="B240">
-        <v>14457.0498046875</v>
-      </c>
-      <c r="C240">
-        <v>1650</v>
+        <v>300</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="2">
-        <v>44274.38818287037</v>
+        <v>44293.38818287037</v>
       </c>
       <c r="B241">
-        <v>14454.099609375</v>
+        <v>14781.150390625</v>
       </c>
       <c r="C241">
-        <v>3150</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="2">
+        <v>44293.38819444444</v>
+      </c>
+      <c r="B242">
+        <v>14782.2001953125</v>
+      </c>
+      <c r="C242">
+        <v>2250</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="2">
-        <v>44274.38820601852</v>
+        <v>44293.38820601852</v>
       </c>
       <c r="B243">
-        <v>14454.97509765625</v>
+        <v>14783</v>
       </c>
       <c r="C243">
-        <v>3600</v>
+        <v>600</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="2">
-        <v>44274.38821759259</v>
+        <v>44293.38821759259</v>
       </c>
       <c r="B244">
-        <v>14453.75</v>
+        <v>14783</v>
       </c>
       <c r="C244">
-        <v>1200</v>
+        <v>450</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="2">
-        <v>44274.38822916667</v>
+        <v>44293.38822916667</v>
       </c>
       <c r="B245">
-        <v>14452</v>
+        <v>14781.5</v>
       </c>
       <c r="C245">
-        <v>2175</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="2">
+        <v>44293.38824074074</v>
+      </c>
+      <c r="B246">
+        <v>14780.150390625</v>
+      </c>
+      <c r="C246">
+        <v>150</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="2">
-        <v>44274.38825231481</v>
+        <v>44293.38825231481</v>
       </c>
       <c r="B247">
-        <v>14451.5</v>
+        <v>14778.2001953125</v>
       </c>
       <c r="C247">
-        <v>2025</v>
+        <v>225</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="2">
-        <v>44274.38826388889</v>
+        <v>44293.38826388889</v>
       </c>
       <c r="B248">
-        <v>14451.5</v>
+        <v>14780</v>
       </c>
       <c r="C248">
-        <v>1650</v>
+        <v>600</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="2">
-        <v>44274.38827546296</v>
+        <v>44293.38827546296</v>
       </c>
       <c r="B249">
-        <v>14452.099609375</v>
+        <v>14780.0498046875</v>
       </c>
       <c r="C249">
-        <v>1125</v>
+        <v>150</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" s="2">
-        <v>44274.38828703704</v>
+        <v>44293.38828703704</v>
       </c>
       <c r="B250">
-        <v>14451.2998046875</v>
+        <v>14780.900390625</v>
       </c>
       <c r="C250">
-        <v>1425</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="2">
-        <v>44274.38829861111</v>
+        <v>44293.38829861111</v>
       </c>
       <c r="B251">
-        <v>14451.099609375</v>
+        <v>14778.5498046875</v>
       </c>
       <c r="C251">
-        <v>900</v>
+        <v>75</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="2">
-        <v>44274.38831018518</v>
+        <v>44293.38831018518</v>
       </c>
       <c r="B252">
-        <v>14451</v>
+        <v>14779.9501953125</v>
       </c>
       <c r="C252">
-        <v>3900</v>
+        <v>600</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" s="2">
-        <v>44274.38832175926</v>
+        <v>44293.38832175926</v>
       </c>
       <c r="B253">
-        <v>14450.099609375</v>
+        <v>14778.5498046875</v>
       </c>
       <c r="C253">
-        <v>1650</v>
+        <v>300</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" s="2">
-        <v>44274.38833333334</v>
+        <v>44293.38833333334</v>
       </c>
       <c r="B254">
-        <v>14450.9501953125</v>
+        <v>14780</v>
       </c>
       <c r="C254">
-        <v>750</v>
+        <v>375</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" s="2">
-        <v>44274.38834490741</v>
+        <v>44293.38834490741</v>
       </c>
       <c r="B255">
-        <v>14451</v>
+        <v>14779</v>
       </c>
       <c r="C255">
-        <v>525</v>
+        <v>450</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="2">
-        <v>44274.38835648148</v>
+        <v>44293.38835648148</v>
       </c>
       <c r="B256">
-        <v>14450</v>
+        <v>14779.0498046875</v>
       </c>
       <c r="C256">
-        <v>5325</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="2">
-        <v>44274.38836805556</v>
+        <v>44293.38836805556</v>
       </c>
       <c r="B257">
-        <v>14450</v>
+        <v>14781.25</v>
       </c>
       <c r="C257">
-        <v>1575</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="2">
-        <v>44274.38837962963</v>
+        <v>44293.38837962963</v>
       </c>
       <c r="B258">
-        <v>14451</v>
+        <v>14779.5</v>
       </c>
       <c r="C258">
-        <v>2175</v>
+        <v>450</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="2">
-        <v>44274.38839120371</v>
+        <v>44293.38839120371</v>
       </c>
       <c r="B259">
-        <v>14450.5</v>
+        <v>14780</v>
       </c>
       <c r="C259">
-        <v>4425</v>
+        <v>375</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="2">
-        <v>44274.38840277777</v>
+        <v>44293.38840277777</v>
       </c>
       <c r="B260">
-        <v>14448</v>
+        <v>14778</v>
       </c>
       <c r="C260">
-        <v>3975</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="2">
+        <v>44293.38841435185</v>
+      </c>
+      <c r="B261">
+        <v>14777.2001953125</v>
+      </c>
+      <c r="C261">
+        <v>2625</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="2">
-        <v>44274.38842592593</v>
+        <v>44293.38842592593</v>
       </c>
       <c r="B262">
-        <v>14446.94970703125</v>
+        <v>14777.2001953125</v>
       </c>
       <c r="C262">
-        <v>5175</v>
+        <v>375</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" s="2">
-        <v>44274.3884375</v>
+        <v>44293.3884375</v>
       </c>
       <c r="B263">
-        <v>14442.7998046875</v>
+        <v>14778.2001953125</v>
       </c>
       <c r="C263">
-        <v>3375</v>
+        <v>75</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="2">
-        <v>44274.38844907407</v>
+        <v>44293.38844907407</v>
       </c>
       <c r="B264">
-        <v>14441.900390625</v>
+        <v>14777.5</v>
       </c>
       <c r="C264">
-        <v>2400</v>
+        <v>675</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" s="2">
-        <v>44274.38846064815</v>
+        <v>44293.38846064815</v>
       </c>
       <c r="B265">
-        <v>14440.0498046875</v>
+        <v>14775.0498046875</v>
       </c>
       <c r="C265">
-        <v>1725</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" s="2">
-        <v>44274.38847222222</v>
+        <v>44293.38847222222</v>
       </c>
       <c r="B266">
-        <v>14440</v>
+        <v>14775.5498046875</v>
       </c>
       <c r="C266">
-        <v>2325</v>
+        <v>75</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" s="2">
-        <v>44274.3884837963</v>
+        <v>44293.3884837963</v>
       </c>
       <c r="B267">
-        <v>14442.400390625</v>
+        <v>14775.0498046875</v>
       </c>
       <c r="C267">
-        <v>1950</v>
+        <v>825</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="2">
+        <v>44293.38849537037</v>
+      </c>
+      <c r="B268">
+        <v>14776.5498046875</v>
+      </c>
+      <c r="C268">
+        <v>1800</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="2">
-        <v>44274.38850694444</v>
+        <v>44293.38850694444</v>
       </c>
       <c r="B269">
-        <v>14442.7998046875</v>
+        <v>14776</v>
       </c>
       <c r="C269">
-        <v>5100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" s="2">
-        <v>44274.38851851852</v>
+        <v>44293.38851851852</v>
       </c>
       <c r="B270">
-        <v>14445.900390625</v>
+        <v>14778</v>
       </c>
       <c r="C270">
-        <v>1575</v>
+        <v>300</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="2">
-        <v>44274.38853009259</v>
+        <v>44293.38853009259</v>
       </c>
       <c r="B271">
-        <v>14445.9501953125</v>
+        <v>14776</v>
       </c>
       <c r="C271">
-        <v>1725</v>
+        <v>150</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="2">
-        <v>44274.38854166667</v>
+        <v>44293.38854166667</v>
       </c>
       <c r="B272">
-        <v>14449.150390625</v>
+        <v>14776</v>
       </c>
       <c r="C272">
-        <v>825</v>
+        <v>75</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" s="2">
-        <v>44274.38855324074</v>
+        <v>44293.38855324074</v>
       </c>
       <c r="B273">
-        <v>14447.900390625</v>
+        <v>14777.2001953125</v>
       </c>
       <c r="C273">
-        <v>1125</v>
+        <v>375</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" s="2">
-        <v>44274.38856481481</v>
+        <v>44293.38856481481</v>
       </c>
       <c r="B274">
-        <v>14446.349609375</v>
+        <v>14778</v>
       </c>
       <c r="C274">
-        <v>1950</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" s="2">
+        <v>44293.38857638889</v>
+      </c>
+      <c r="B275">
+        <v>14778</v>
+      </c>
+      <c r="C275">
+        <v>750</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" s="2">
-        <v>44274.38858796296</v>
+        <v>44293.38858796296</v>
       </c>
       <c r="B276">
-        <v>14446.5</v>
+        <v>14777</v>
       </c>
       <c r="C276">
-        <v>2625</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" s="2">
-        <v>44274.38859953704</v>
+        <v>44293.38859953704</v>
       </c>
       <c r="B277">
-        <v>14443.849609375</v>
+        <v>14780</v>
       </c>
       <c r="C277">
-        <v>2325</v>
+        <v>675</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="2">
+        <v>44293.38861111111</v>
+      </c>
+      <c r="B278">
+        <v>14779.599609375</v>
+      </c>
+      <c r="C278">
+        <v>450</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="2">
-        <v>44274.38862268518</v>
+        <v>44293.38862268518</v>
       </c>
       <c r="B279">
-        <v>14441</v>
+        <v>14779.599609375</v>
       </c>
       <c r="C279">
-        <v>1950</v>
+        <v>375</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="2">
-        <v>44274.38863425926</v>
+        <v>44293.38863425926</v>
       </c>
       <c r="B280">
-        <v>14442.22509765625</v>
+        <v>14780.099609375</v>
       </c>
       <c r="C280">
-        <v>3150</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" s="2">
+        <v>44293.38864583334</v>
+      </c>
+      <c r="B281">
+        <v>14780</v>
+      </c>
+      <c r="C281">
+        <v>1050</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="2">
-        <v>44274.38865740741</v>
+        <v>44293.38865740741</v>
       </c>
       <c r="B282">
-        <v>14440</v>
+        <v>14780</v>
       </c>
       <c r="C282">
-        <v>2250</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="2">
-        <v>44274.38866898148</v>
+        <v>44293.38866898148</v>
       </c>
       <c r="B283">
-        <v>14443</v>
+        <v>14781.7001953125</v>
       </c>
       <c r="C283">
-        <v>2025</v>
+        <v>75</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="2">
-        <v>44274.38868055555</v>
+        <v>44293.38868055555</v>
       </c>
       <c r="B284">
-        <v>14440</v>
+        <v>14778.0498046875</v>
       </c>
       <c r="C284">
-        <v>3600</v>
+        <v>525</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="2">
-        <v>44274.38869212963</v>
+        <v>44293.38869212963</v>
       </c>
       <c r="B285">
-        <v>14440.599609375</v>
+        <v>14777.650390625</v>
       </c>
       <c r="C285">
-        <v>1050</v>
+        <v>600</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" s="2">
-        <v>44274.38870370371</v>
+        <v>44293.38870370371</v>
       </c>
       <c r="B286">
-        <v>14437.0498046875</v>
+        <v>14780.0498046875</v>
       </c>
       <c r="C286">
-        <v>2400</v>
+        <v>675</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" s="2">
-        <v>44274.38871527778</v>
+        <v>44293.38871527778</v>
       </c>
       <c r="B287">
-        <v>14438.099609375</v>
+        <v>14782.099609375</v>
       </c>
       <c r="C287">
-        <v>1800</v>
+        <v>975</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" s="2">
-        <v>44274.38872685185</v>
+        <v>44293.38872685185</v>
       </c>
       <c r="B288">
-        <v>14442.099609375</v>
+        <v>14784.0498046875</v>
       </c>
       <c r="C288">
-        <v>2100</v>
+        <v>750</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="2">
-        <v>44274.38873842593</v>
+        <v>44293.38873842593</v>
       </c>
       <c r="B289">
-        <v>14439.849609375</v>
+        <v>14782.5498046875</v>
       </c>
       <c r="C289">
-        <v>1575</v>
+        <v>600</v>
       </c>
     </row>
     <row r="290" spans="1:3">
       <c r="A290" s="2">
-        <v>44274.38875</v>
+        <v>44293.38875</v>
       </c>
       <c r="B290">
-        <v>14442.349609375</v>
+        <v>14781.7998046875</v>
       </c>
       <c r="C290">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3">
-      <c r="A291" s="2">
-        <v>44274.38876157408</v>
-      </c>
-      <c r="B291">
-        <v>14444.099609375</v>
-      </c>
-      <c r="C291">
-        <v>2475</v>
+        <v>75</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" s="2">
-        <v>44274.38877314814</v>
+        <v>44293.38877314814</v>
       </c>
       <c r="B292">
-        <v>14443.2001953125</v>
+        <v>14782.5</v>
       </c>
       <c r="C292">
-        <v>1875</v>
+        <v>75</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" s="2">
-        <v>44274.38878472222</v>
+        <v>44293.38878472222</v>
       </c>
       <c r="B293">
-        <v>14442.25</v>
+        <v>14783.7998046875</v>
       </c>
       <c r="C293">
-        <v>3300</v>
+        <v>75</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="2">
-        <v>44274.3887962963</v>
+        <v>44293.3887962963</v>
       </c>
       <c r="B294">
-        <v>14440.400390625</v>
+        <v>14783</v>
       </c>
       <c r="C294">
-        <v>9000</v>
+        <v>675</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="A295" s="2">
-        <v>44274.38880787037</v>
+        <v>44293.38880787037</v>
       </c>
       <c r="B295">
-        <v>14440.2998046875</v>
+        <v>14784.900390625</v>
       </c>
       <c r="C295">
-        <v>1800</v>
+        <v>150</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" s="2">
-        <v>44274.38881944444</v>
+        <v>44293.38881944444</v>
       </c>
       <c r="B296">
-        <v>14440.0498046875</v>
+        <v>14783.7998046875</v>
       </c>
       <c r="C296">
-        <v>1575</v>
+        <v>225</v>
       </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" s="2">
-        <v>44274.38883101852</v>
+        <v>44293.38883101852</v>
       </c>
       <c r="B297">
-        <v>14440</v>
+        <v>14781.349609375</v>
       </c>
       <c r="C297">
-        <v>1125</v>
+        <v>750</v>
       </c>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="2">
-        <v>44274.38884259259</v>
+        <v>44293.38884259259</v>
       </c>
       <c r="B298">
-        <v>14438.25</v>
+        <v>14782.650390625</v>
       </c>
       <c r="C298">
-        <v>2925</v>
+        <v>150</v>
       </c>
     </row>
     <row r="299" spans="1:3">
       <c r="A299" s="2">
-        <v>44274.38885416667</v>
+        <v>44293.38885416667</v>
       </c>
       <c r="B299">
-        <v>14438.5498046875</v>
+        <v>14782.7001953125</v>
       </c>
       <c r="C299">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3">
-      <c r="A300" s="2">
-        <v>44274.38886574074</v>
-      </c>
-      <c r="B300">
-        <v>14438.5498046875</v>
-      </c>
-      <c r="C300">
-        <v>2175</v>
+        <v>525</v>
       </c>
     </row>
     <row r="301" spans="1:3">
       <c r="A301" s="2">
-        <v>44274.38887731481</v>
+        <v>44293.38887731481</v>
       </c>
       <c r="B301">
-        <v>14438</v>
+        <v>14782.349609375</v>
       </c>
       <c r="C301">
-        <v>6375</v>
+        <v>675</v>
       </c>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="2">
-        <v>44274.38888888889</v>
+        <v>44293.38888888889</v>
       </c>
       <c r="B302">
-        <v>14440.25</v>
+        <v>14790</v>
       </c>
       <c r="C302">
-        <v>975</v>
+        <v>11850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>